<commit_message>
FIXED TRANSITIONS AND NET REVENUE
</commit_message>
<xml_diff>
--- a/PEWI Budgets 2024$ - 2025$ (021425).xlsx
+++ b/PEWI Budgets 2024$ - 2025$ (021425).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_pewi\pewi3.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EE32D1-59D1-4421-96C0-3FFC9638EBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8295792B-1A7B-437F-90D3-F70EBA989AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" activeTab="1" xr2:uid="{2A59C1DF-064D-264D-B5F5-440AD859B569}"/>
+    <workbookView minimized="1" xWindow="3870" yWindow="660" windowWidth="21600" windowHeight="13185" activeTab="7" xr2:uid="{2A59C1DF-064D-264D-B5F5-440AD859B569}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions &amp; summary data" sheetId="19" r:id="rId1"/>
@@ -2152,7 +2152,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="51">
+  <fonts count="52">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2497,6 +2497,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -3209,7 +3216,7 @@
     <xf numFmtId="7" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="519">
+  <cellXfs count="520">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -4329,6 +4336,15 @@
     <xf numFmtId="44" fontId="0" fillId="12" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4350,21 +4366,12 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4377,6 +4384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="51" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -5226,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1E20D6-F156-C447-BE27-5EDB562A8E09}">
   <dimension ref="B2:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -8197,16 +8205,16 @@
       <c r="L3" s="492"/>
     </row>
     <row r="4" spans="2:12" ht="33.75">
-      <c r="B4" s="503" t="s">
+      <c r="B4" s="506" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="504"/>
-      <c r="D4" s="504"/>
-      <c r="E4" s="504"/>
-      <c r="F4" s="504"/>
-      <c r="G4" s="504"/>
-      <c r="H4" s="504"/>
-      <c r="I4" s="505"/>
+      <c r="C4" s="507"/>
+      <c r="D4" s="507"/>
+      <c r="E4" s="507"/>
+      <c r="F4" s="507"/>
+      <c r="G4" s="507"/>
+      <c r="H4" s="507"/>
+      <c r="I4" s="508"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" thickBot="1">
       <c r="B5" s="145" t="s">
@@ -8227,10 +8235,10 @@
       <c r="G5" s="146" t="s">
         <v>200</v>
       </c>
-      <c r="H5" s="506" t="s">
+      <c r="H5" s="509" t="s">
         <v>201</v>
       </c>
-      <c r="I5" s="507"/>
+      <c r="I5" s="510"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" thickBot="1">
       <c r="B6" s="147"/>
@@ -8308,10 +8316,10 @@
       <c r="G9" s="150" t="s">
         <v>200</v>
       </c>
-      <c r="H9" s="508" t="s">
+      <c r="H9" s="511" t="s">
         <v>212</v>
       </c>
-      <c r="I9" s="509"/>
+      <c r="I9" s="512"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="151" t="s">
@@ -8335,11 +8343,11 @@
         <f>F10/C6</f>
         <v>160</v>
       </c>
-      <c r="H10" s="510">
+      <c r="H10" s="503">
         <f>G10/$I$7</f>
         <v>290.90909090909088</v>
       </c>
-      <c r="I10" s="511"/>
+      <c r="I10" s="504"/>
     </row>
     <row r="11" spans="2:12" ht="17.25">
       <c r="B11" s="157" t="s">
@@ -8363,11 +8371,11 @@
         <f>F11/20</f>
         <v>0</v>
       </c>
-      <c r="H11" s="512">
+      <c r="H11" s="513">
         <f>G11/$I$7</f>
         <v>0</v>
       </c>
-      <c r="I11" s="513"/>
+      <c r="I11" s="514"/>
     </row>
     <row r="12" spans="2:12" ht="17.25">
       <c r="B12" s="151" t="s">
@@ -8816,11 +8824,11 @@
         <f>G26+G6+G30</f>
         <v>3496.809836065574</v>
       </c>
-      <c r="H31" s="510">
+      <c r="H31" s="503">
         <f t="shared" si="0"/>
         <v>5.2981967213114753</v>
       </c>
-      <c r="I31" s="511"/>
+      <c r="I31" s="504"/>
       <c r="J31" t="s">
         <v>242</v>
       </c>
@@ -8862,11 +8870,11 @@
       <c r="I33" s="168"/>
     </row>
     <row r="34" spans="1:12" ht="17.25">
-      <c r="B34" s="514" t="s">
+      <c r="B34" s="505" t="s">
         <v>245</v>
       </c>
-      <c r="C34" s="514"/>
-      <c r="D34" s="514"/>
+      <c r="C34" s="505"/>
+      <c r="D34" s="505"/>
       <c r="L34">
         <f>50/H38</f>
         <v>2.1917808219178081</v>
@@ -8903,11 +8911,13 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="K2:L3"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
@@ -8920,13 +8930,11 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K2:L3"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="B34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" xr:uid="{F7409163-740C-D24A-84CB-4E3439D40069}"/>
@@ -8967,16 +8975,16 @@
       <c r="L3" s="492"/>
     </row>
     <row r="4" spans="2:12" ht="33.75">
-      <c r="B4" s="503" t="s">
+      <c r="B4" s="506" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="504"/>
-      <c r="D4" s="504"/>
-      <c r="E4" s="504"/>
-      <c r="F4" s="504"/>
-      <c r="G4" s="504"/>
-      <c r="H4" s="504"/>
-      <c r="I4" s="505"/>
+      <c r="C4" s="507"/>
+      <c r="D4" s="507"/>
+      <c r="E4" s="507"/>
+      <c r="F4" s="507"/>
+      <c r="G4" s="507"/>
+      <c r="H4" s="507"/>
+      <c r="I4" s="508"/>
     </row>
     <row r="5" spans="2:12" ht="16.5" thickBot="1">
       <c r="B5" s="145" t="s">
@@ -8997,10 +9005,10 @@
       <c r="G5" s="146" t="s">
         <v>200</v>
       </c>
-      <c r="H5" s="506" t="s">
+      <c r="H5" s="509" t="s">
         <v>201</v>
       </c>
-      <c r="I5" s="507"/>
+      <c r="I5" s="510"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" thickBot="1">
       <c r="B6" s="147"/>
@@ -9078,10 +9086,10 @@
       <c r="G9" s="150" t="s">
         <v>200</v>
       </c>
-      <c r="H9" s="508" t="s">
+      <c r="H9" s="511" t="s">
         <v>212</v>
       </c>
-      <c r="I9" s="509"/>
+      <c r="I9" s="512"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="151" t="s">
@@ -9105,11 +9113,11 @@
         <f>F10/C6</f>
         <v>160</v>
       </c>
-      <c r="H10" s="510" t="e">
+      <c r="H10" s="503" t="e">
         <f>G10/$J$7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="511"/>
+      <c r="I10" s="504"/>
     </row>
     <row r="11" spans="2:12" ht="17.25">
       <c r="B11" s="157" t="s">
@@ -9133,11 +9141,11 @@
         <f>F11/20</f>
         <v>0</v>
       </c>
-      <c r="H11" s="512" t="e">
+      <c r="H11" s="513" t="e">
         <f t="shared" ref="H11" si="0">G11/$J$7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="513"/>
+      <c r="I11" s="514"/>
     </row>
     <row r="12" spans="2:12" ht="17.25">
       <c r="B12" s="151" t="s">
@@ -9612,11 +9620,11 @@
         <f>G27+G6+G31</f>
         <v>3556.809836065574</v>
       </c>
-      <c r="H32" s="510">
+      <c r="H32" s="503">
         <f t="shared" si="1"/>
         <v>5.3891058122205671</v>
       </c>
-      <c r="I32" s="511"/>
+      <c r="I32" s="504"/>
       <c r="J32" t="s">
         <v>242</v>
       </c>
@@ -9658,11 +9666,11 @@
       <c r="I34" s="168"/>
     </row>
     <row r="35" spans="1:9" ht="17.25">
-      <c r="B35" s="514" t="s">
+      <c r="B35" s="505" t="s">
         <v>245</v>
       </c>
-      <c r="C35" s="514"/>
-      <c r="D35" s="514"/>
+      <c r="C35" s="505"/>
+      <c r="D35" s="505"/>
     </row>
     <row r="36" spans="1:9" ht="17.25">
       <c r="B36" s="174" t="s">
@@ -9683,16 +9691,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
     <mergeCell ref="K2:L3"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H28:I28"/>
@@ -9708,6 +9706,16 @@
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L8" r:id="rId1" xr:uid="{C10CBC37-B907-284D-A5CD-D379AFEFC3CE}"/>
@@ -13721,7 +13729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E4A553-5A20-544F-981B-7A427BC0DBF5}">
   <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -16862,7 +16870,7 @@
     <row r="77" spans="1:10">
       <c r="A77" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -19590,7 +19598,7 @@
     <row r="101" spans="1:11">
       <c r="A101" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -21205,7 +21213,7 @@
     <row r="73" spans="1:11">
       <c r="A73" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -22984,7 +22992,7 @@
     <row r="88" spans="1:11">
       <c r="A88" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -25966,7 +25974,7 @@
     <row r="133" spans="1:11">
       <c r="A133" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -26026,8 +26034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1811BFB6-13E6-734C-8B47-C560968C2226}">
   <dimension ref="A1:O138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:M7"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -28714,7 +28722,7 @@
         <f>((H113*H79)+H70)/(D9+(C80*C79))</f>
         <v>26.401052631578946</v>
       </c>
-      <c r="I120" s="29">
+      <c r="I120" s="519">
         <f>((I113*H79)+I70)/(D9+(C80*C79))</f>
         <v>63.445185824561399</v>
       </c>
@@ -28929,7 +28937,7 @@
     <row r="133" spans="1:11">
       <c r="A133" s="86">
         <f ca="1">TODAY()</f>
-        <v>45707</v>
+        <v>45781</v>
       </c>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -28981,7 +28989,8 @@
     <hyperlink ref="L6:M7" location="'Instructions &amp; summary data'!A1" display="Return to instructions page" xr:uid="{5FA1D311-4293-5543-9CC2-42C5D90C1D94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>